<commit_message>
add - management command - sales_saleinvoicecategory, sales_saleinvoiceheader
</commit_message>
<xml_diff>
--- a/core/seed_customers_customer.xlsx
+++ b/core/seed_customers_customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1F8D39-F2BA-4E9E-94E2-7C683047638A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8187589-BF57-4AEF-BE07-8C3B4C4B3F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>PATIENT</t>
+  </si>
+  <si>
+    <t>CUSTOMER ID</t>
+  </si>
+  <si>
+    <t>cust 01</t>
+  </si>
+  <si>
+    <t>cust 02</t>
+  </si>
+  <si>
+    <t>cust 03</t>
+  </si>
+  <si>
+    <t>cust 04</t>
+  </si>
+  <si>
+    <t>cust 05</t>
+  </si>
+  <si>
+    <t>cust 06</t>
+  </si>
+  <si>
+    <t>cust 07</t>
   </si>
 </sst>
 </file>
@@ -935,123 +959,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>